<commit_message>
updated citations of progress noutes
</commit_message>
<xml_diff>
--- a/mapping/mml_progress_course_mapping.xlsx
+++ b/mapping/mml_progress_course_mapping.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="190">
   <si>
     <t>Archetype</t>
     <phoneticPr fontId="1"/>
@@ -527,22 +527,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>/content[openEHR-EHR-SECTION.soap.v1 and name/value='SOAP']/items[at0002]/items[openEHR-EHR-OBSERVATION.exam.v1 and name/value='Physical examination findings']/protocol[at0007]/items[openEHR-EHR-CLUSTER.citation.v1 and name/value='Citation']/items[at0002]/value</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>/content[openEHR-EHR-SECTION.soap.v1 and name/value='SOAP']/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='RxRecord']/items[openEHR-EHR-EVALUATION.citation.v1 and name/value='Citation']/data[at0001]/items[openEHR-EHR-CLUSTER.citation.v1 and name/value='Citation']/items[at0002]/value</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>/content[openEHR-EHR-SECTION.soap.v1 and name/value='SOAP']/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='TxRecord']/items[openEHR-EHR-OBSERVATION.progress_note.v1 and name/value='Progress Note']/data[at0001]/events[at0002]/data[at0003]/items[at0004]/value</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>/content[openEHR-EHR-SECTION.soap.v1 and name/value='SOAP']/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='TxRecord']/items[openEHR-EHR-EVALUATION.citation.v1 and name/value='Citation ']/data[at0001]/items[openEHR-EHR-CLUSTER.citation.v1 and name/value='Citation']/items[at0002]/value</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>/content[openEHR-EHR-SECTION.soap.v1 and name/value='SOAP']/items[at0003]/items[openEHR-EHR-EVALUATION.clinical_synopsis.v1 and name/value='Clinical Synopsis']/data[at0001]/items[at0002]/value</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -559,10 +547,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>/content[openEHR-EHR-SECTION.soap.v1 and name/value='SOAP']/items[at0004]/items[openEHR-EHR-INSTRUCTION.request.v1 and name/value='testOrder']/protocol[at0008]/items[openEHR-EHR-CLUSTER.citation.v1 and name/value='Citation']/items[at0002]/value</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Description</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -571,10 +555,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>/content[openEHR-EHR-SECTION.soap.v1 and name/value='SOAP']/items[at0004]/items[openEHR-EHR-INSTRUCTION.request.v1 and name/value='RxOrder']/protocol[at0008]/items[openEHR-EHR-CLUSTER.citation.v1 and name/value='Citation']/items[at0002]/value</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>/content[openEHR-EHR-SECTION.soap.v1 and name/value='SOAP']/items[at0004]/items[openEHR-EHR-INSTRUCTION.request.v1 and name/value='RxOrder']/activities[at0001 and name/value='Request']/description[at0009]/items[at0121]/value</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -591,10 +571,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>/content[openEHR-EHR-SECTION.soap.v1 and name/value='SOAP']/items[at0004]/items[openEHR-EHR-INSTRUCTION.request.v1 and name/value='TxOrder']/protocol[at0008]/items[openEHR-EHR-CLUSTER.citation.v1 and name/value='Citation']/items[at0002]/value</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>/content[openEHR-EHR-SECTION.soap.v1 and name/value='SOAP']/items[at0004]/items[openEHR-EHR-INSTRUCTION.care_plan.v1 and name/value='Care Plan']/activities[at0001]/description[at0004]/items[at0007]/value</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -651,6 +627,118 @@
   </si>
   <si>
     <t>/content[openEHR-EHR-EVALUATION.citation.v1]/data[at0001]/items[openEHR-EHR-CLUSTER.citation.v1]/items[at0002]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-OBSERVATION.exam.v1]/data[at0001]/events/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-OBSERVATION.exam.v1]/data[at0001]/events[at0002]/data[at0003]/items[openEHR-EHR-CLUSTER.citation.v1]/items[at0001][at0002]/data[at0003]/items[openEHR-EHR-CLUSTER.citation.v1]/items[at0001]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-OBSERVATION.exam.v1]/data[at0001]/events[at0002]/data[at0003]/items[openEHR-EHR-CLUSTER.citation.v1]/items[at0004]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-OBSERVATION.exam.v1]/data[at0001]/events[at0002]/data[at0003]/items[openEHR-EHR-CLUSTER.citation.v1]/items[at0003]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-OBSERVATION.exam.v1]/data[at0001]/events[at0002]/data[at0003]/items[openEHR-EHR-CLUSTER.citation.v1]/items[at0002]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='Test result']/items[openEHR-EHR-EVALUATION.citation.v1]/data[at0001]/items[openEHR-EHR-CLUSTER.citation.v1]/items[at0001]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='Test result']/items[openEHR-EHR-EVALUATION.citation.v1]/data[at0001]/items[openEHR-EHR-CLUSTER.citation.v1]/items[at0004]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='Test result']/items[openEHR-EHR-EVALUATION.citation.v1]/data[at0001]/items[openEHR-EHR-CLUSTER.citation.v1]/items[at0003]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='Test result']/items[openEHR-EHR-EVALUATION.citation.v1]/data[at0001]/items[openEHR-EHR-CLUSTER.citation.v1]/items[at0002]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='RxRecord']/items[openEHR-EHR-EVALUATION.citation.v1]/data[at0001]/items[openEHR-EHR-CLUSTER.citation.v1]/items[at0003]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='RxRecord']/items[openEHR-EHR-EVALUATION.citation.v1]/data[at0001]/items[openEHR-EHR-CLUSTER.citation.v1]/items[at0001]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='RxRecord']/items[openEHR-EHR-EVALUATION.citation.v1]/data[at0001]/items[openEHR-EHR-CLUSTER.citation.v1]/items[at0004]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='TxRecord']/items[openEHR-EHR-EVALUATION.citation.v1]/data[at0001]/items[openEHR-EHR-CLUSTER.citation.v1]/items[at0001]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='TxRecord']/items[openEHR-EHR-EVALUATION.citation.v1]/data[at0001]/items[openEHR-EHR-CLUSTER.citation.v1]/items[at0004]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='TxRecord']/items[openEHR-EHR-EVALUATION.citation.v1]/data[at0001]/items[openEHR-EHR-CLUSTER.citation.v1]/items[at0003]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='TxRecord']/items[openEHR-EHR-EVALUATION.citation.v1]/data[at0001]/items[openEHR-EHR-CLUSTER.citation.v1]/items[at0002]va;ue</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0002]/items[openEHR-EHR-SECTION.adhoc.v1]/items[openEHR-EHR-SECTION.adhoc.v1 and name/value='RxRecord']/items[openEHR-EHR-EVALUATION.citation.v1]/data[at0001]/items[openEHR-EHR-CLUSTER.citation.v1]/items[at0002]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-INSTRUCTION.request.v1 and name/value='testOrder']/activities[at0001]/description[at0009]/items[openEHR-EHR-CLUSTER.citation.v1]/items[at0003]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-INSTRUCTION.request.v1 and name/value='testOrder']/activities[at0001]/description[at0009]/items[openEHR-EHR-CLUSTER.citation.v1]/items[at0002]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-INSTRUCTION.request.v1 and name/value='testOrder']/activities[at0001]/description[at0009]/items[openEHR-EHR-CLUSTER.citation.v1]/items[at0001]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-INSTRUCTION.request.v1 and name/value='testOrder']/activities[at0001]/description[at0009]/items[openEHR-EHR-CLUSTER.citation.v1]/items[at0004]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-INSTRUCTION.request.v1 and name/value='RxOrder']/activities[at0001]/description[at0009]/items[openEHR-EHR-CLUSTER.citation.v1]/items[at0002]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-INSTRUCTION.request.v1 and name/value='RxOrder']/activities[at0001]/description[at0009]/items[openEHR-EHR-CLUSTER.citation.v1]/items[at0001]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-INSTRUCTION.request.v1 and name/value='RxOrder']/activities[at0001]/description[at0009]/items[openEHR-EHR-CLUSTER.citation.v1]/items[at0004]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-INSTRUCTION.request.v1 and name/value='RxOrder']/activities[at0001]/description[at0009]/items[openEHR-EHR-CLUSTER.citation.v1]/items[at0003]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-INSTRUCTION.request.v1 and name/value='TxOrder']/activities[at0001]/description[at0009]/items[openEHR-EHR-CLUSTER.citation.v1]/items[at0002]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-INSTRUCTION.request.v1 and name/value='TxOrder']/activities[at0001]/description[at0009]/items[openEHR-EHR-CLUSTER.citation.v1]/items[at0001]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-INSTRUCTION.request.v1 and name/value='TxOrder']/activities[at0001]/description[at0009]/items[openEHR-EHR-CLUSTER.citation.v1]/items[at0004]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.soap.v1]/items[at0004]/items[openEHR-EHR-INSTRUCTION.request.v1 and name/value='TxOrder']/activities[at0001]/description[at0009]/items[openEHR-EHR-CLUSTER.citation.v1]/items[at0003]/value</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1076,10 +1164,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K53"/>
+  <dimension ref="A1:K82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K75" sqref="K75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1193,7 +1281,7 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>7</v>
@@ -1204,19 +1292,19 @@
       <c r="E7" s="7"/>
       <c r="F7" s="8"/>
       <c r="I7" s="9" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="K7" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>7</v>
@@ -1227,19 +1315,19 @@
       <c r="E8" s="7"/>
       <c r="F8" s="8"/>
       <c r="I8" s="4" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="J8" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="K8" t="s">
         <v>159</v>
-      </c>
-      <c r="K8" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>7</v>
@@ -1250,25 +1338,25 @@
       <c r="E9" s="7"/>
       <c r="F9" s="8"/>
       <c r="I9" s="4" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K9" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="8"/>
@@ -1279,7 +1367,7 @@
         <v>129</v>
       </c>
       <c r="K10" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1439,7 +1527,7 @@
         <v>116</v>
       </c>
       <c r="K18" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1667,130 +1755,105 @@
       <c r="H29" t="s">
         <v>102</v>
       </c>
-      <c r="I29" t="s">
-        <v>103</v>
-      </c>
-      <c r="J29" t="s">
-        <v>129</v>
-      </c>
-      <c r="K29" t="s">
-        <v>135</v>
-      </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>53</v>
-      </c>
+      <c r="A30" s="3"/>
       <c r="B30" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C30" s="3"/>
+        <v>148</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="D30" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F30" s="3"/>
-      <c r="H30" t="s">
-        <v>99</v>
-      </c>
-      <c r="I30" s="4" t="s">
-        <v>101</v>
+        <v>25</v>
+      </c>
+      <c r="E30" s="7"/>
+      <c r="F30" s="8"/>
+      <c r="I30" s="9" t="s">
+        <v>149</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>113</v>
+        <v>150</v>
       </c>
       <c r="K30" t="s">
-        <v>131</v>
+        <v>162</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="A31" s="3"/>
       <c r="B31" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F31" s="3"/>
-      <c r="H31" t="s">
-        <v>102</v>
-      </c>
-      <c r="I31" t="s">
-        <v>103</v>
-      </c>
-      <c r="J31" t="s">
-        <v>132</v>
+        <v>151</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E31" s="7"/>
+      <c r="F31" s="8"/>
+      <c r="I31" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>153</v>
       </c>
       <c r="K31" t="s">
-        <v>130</v>
+        <v>163</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="A32" s="3"/>
       <c r="B32" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C32" s="3"/>
+        <v>154</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="D32" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F32" s="3"/>
-      <c r="H32" t="s">
-        <v>99</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="E32" s="7"/>
+      <c r="F32" s="8"/>
       <c r="I32" s="4" t="s">
-        <v>101</v>
+        <v>155</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>116</v>
+        <v>156</v>
       </c>
       <c r="K32" t="s">
-        <v>134</v>
+        <v>164</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>58</v>
-      </c>
+      <c r="A33" s="3"/>
       <c r="B33" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F33" s="3"/>
-      <c r="H33" t="s">
-        <v>102</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E33" s="7"/>
+      <c r="F33" s="8"/>
       <c r="I33" t="s">
         <v>103</v>
       </c>
       <c r="J33" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="K33" t="s">
-        <v>136</v>
+        <v>165</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3" t="s">
@@ -1807,15 +1870,15 @@
         <v>101</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="K34" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>19</v>
@@ -1833,117 +1896,135 @@
         <v>103</v>
       </c>
       <c r="J35" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K35" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>62</v>
-      </c>
+      <c r="A36" s="3"/>
       <c r="B36" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E36" s="7"/>
+      <c r="F36" s="8"/>
+      <c r="I36" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="K36" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E37" s="7"/>
+      <c r="F37" s="8"/>
+      <c r="I37" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="K37" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E38" s="7"/>
+      <c r="F38" s="8"/>
+      <c r="I38" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="K38" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E39" s="7"/>
+      <c r="F39" s="8"/>
+      <c r="I39" t="s">
+        <v>103</v>
+      </c>
+      <c r="J39" t="s">
+        <v>129</v>
+      </c>
+      <c r="K39" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F36" s="3"/>
-      <c r="H36" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F37" s="3"/>
-      <c r="I37" t="s">
-        <v>80</v>
-      </c>
-      <c r="J37" t="s">
+      <c r="F40" s="3"/>
+      <c r="H40" t="s">
+        <v>99</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="J40" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="K37" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F38" s="3"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" s="3"/>
-      <c r="H39" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="I39" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="J39" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="K39" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="H40" s="5"/>
-      <c r="I40" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="J40" s="6" t="s">
-        <v>140</v>
-      </c>
       <c r="K40" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>19</v>
@@ -1957,137 +2038,130 @@
       <c r="H41" t="s">
         <v>102</v>
       </c>
-      <c r="I41" t="s">
-        <v>103</v>
-      </c>
-      <c r="J41" t="s">
-        <v>132</v>
-      </c>
-      <c r="K41" t="s">
-        <v>143</v>
-      </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>71</v>
-      </c>
+      <c r="A42" s="3"/>
       <c r="B42" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C42" s="3"/>
+        <v>148</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="D42" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F42" s="3"/>
-      <c r="H42" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="I42" s="4" t="s">
-        <v>144</v>
+        <v>25</v>
+      </c>
+      <c r="E42" s="7"/>
+      <c r="F42" s="8"/>
+      <c r="I42" s="9" t="s">
+        <v>149</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>116</v>
+        <v>150</v>
       </c>
       <c r="K42" t="s">
-        <v>145</v>
+        <v>171</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="H43" s="5"/>
+      <c r="B43" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E43" s="7"/>
+      <c r="F43" s="8"/>
       <c r="I43" s="4" t="s">
-        <v>108</v>
+        <v>152</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>116</v>
+        <v>153</v>
       </c>
       <c r="K43" t="s">
-        <v>147</v>
+        <v>172</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>73</v>
-      </c>
+      <c r="A44" s="3"/>
       <c r="B44" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F44" s="3"/>
-      <c r="H44" t="s">
-        <v>102</v>
-      </c>
-      <c r="I44" t="s">
+        <v>154</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E44" s="7"/>
+      <c r="F44" s="8"/>
+      <c r="I44" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="J44" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="K44" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="3"/>
+      <c r="B45" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E45" s="7"/>
+      <c r="F45" s="8"/>
+      <c r="I45" t="s">
         <v>103</v>
       </c>
-      <c r="J44" s="4" t="s">
+      <c r="J45" t="s">
         <v>133</v>
       </c>
-      <c r="K44" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E45" s="3" t="s">
+      <c r="K45" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E46" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F45" s="3"/>
-      <c r="H45" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="I45" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="J45" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="K45" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
       <c r="F46" s="3"/>
-      <c r="H46" s="5"/>
+      <c r="H46" t="s">
+        <v>99</v>
+      </c>
       <c r="I46" s="4" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="J46" s="4" t="s">
         <v>116</v>
       </c>
       <c r="K46" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>19</v>
@@ -2101,62 +2175,675 @@
       <c r="H47" t="s">
         <v>102</v>
       </c>
-      <c r="I47" t="s">
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="3"/>
+      <c r="B48" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E48" s="7"/>
+      <c r="F48" s="8"/>
+      <c r="I48" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="J48" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="K48" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="3"/>
+      <c r="B49" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E49" s="7"/>
+      <c r="F49" s="8"/>
+      <c r="I49" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="J49" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="K49" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="3"/>
+      <c r="B50" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E50" s="7"/>
+      <c r="F50" s="8"/>
+      <c r="I50" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="J50" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="K50" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="3"/>
+      <c r="B51" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E51" s="7"/>
+      <c r="F51" s="8"/>
+      <c r="I51" t="s">
         <v>103</v>
       </c>
-      <c r="J47" s="4" t="s">
+      <c r="J51" t="s">
         <v>133</v>
       </c>
-      <c r="K47" t="s">
+      <c r="K51" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" s="3"/>
+      <c r="H52" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F53" s="3"/>
+      <c r="I53" t="s">
+        <v>80</v>
+      </c>
+      <c r="J53" t="s">
+        <v>116</v>
+      </c>
+      <c r="K53" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F54" s="3"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F55" s="3"/>
+      <c r="H55" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="I55" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="J55" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="K55" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="3"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="J56" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="K56" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F57" s="3"/>
+      <c r="H57" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="3"/>
+      <c r="B58" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E58" s="7"/>
+      <c r="F58" s="8"/>
+      <c r="I58" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="J58" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="K58" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="3"/>
+      <c r="B59" s="3" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+      <c r="C59" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E59" s="7"/>
+      <c r="F59" s="8"/>
+      <c r="I59" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="J59" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="K59" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" s="3"/>
+      <c r="B60" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E60" s="7"/>
+      <c r="F60" s="8"/>
+      <c r="I60" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="J60" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="K60" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" s="3"/>
+      <c r="B61" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E61" s="7"/>
+      <c r="F61" s="8"/>
+      <c r="I61" t="s">
+        <v>103</v>
+      </c>
+      <c r="J61" t="s">
+        <v>132</v>
+      </c>
+      <c r="K61" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F62" s="3"/>
+      <c r="H62" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="I62" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="J62" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="K62" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" s="3"/>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
+      <c r="H63" s="5"/>
+      <c r="I63" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="J63" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="K63" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F64" s="3"/>
+      <c r="H64" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65" s="3"/>
+      <c r="B65" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E65" s="7"/>
+      <c r="F65" s="8"/>
+      <c r="I65" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="J65" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="K65" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" s="3"/>
+      <c r="B66" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E66" s="7"/>
+      <c r="F66" s="8"/>
+      <c r="I66" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="J66" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="K66" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" s="3"/>
+      <c r="B67" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E67" s="7"/>
+      <c r="F67" s="8"/>
+      <c r="I67" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="J67" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="K67" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68" s="3"/>
+      <c r="B68" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E68" s="7"/>
+      <c r="F68" s="8"/>
+      <c r="I68" t="s">
+        <v>103</v>
+      </c>
+      <c r="J68" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="K68" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F69" s="3"/>
+      <c r="H69" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="I69" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="J69" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="K69" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70" s="3"/>
+      <c r="B70" s="3"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
+      <c r="H70" s="5"/>
+      <c r="I70" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J70" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="K70" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F71" s="3"/>
+      <c r="H71" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A72" s="3"/>
+      <c r="B72" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E72" s="7"/>
+      <c r="F72" s="8"/>
+      <c r="I72" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="J72" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="K72" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73" s="3"/>
+      <c r="B73" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E73" s="7"/>
+      <c r="F73" s="8"/>
+      <c r="I73" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="J73" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="K73" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A74" s="3"/>
+      <c r="B74" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E74" s="7"/>
+      <c r="F74" s="8"/>
+      <c r="I74" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="J74" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="K74" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A75" s="3"/>
+      <c r="B75" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E75" s="7"/>
+      <c r="F75" s="8"/>
+      <c r="I75" t="s">
+        <v>103</v>
+      </c>
+      <c r="J75" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="K75" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A76" s="3"/>
+      <c r="B76" s="3"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
+      <c r="J76" s="4"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B77" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E48" s="3" t="s">
+      <c r="C77" s="3"/>
+      <c r="D77" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E77" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F48" s="3"/>
-      <c r="H48" t="s">
+      <c r="F77" s="3"/>
+      <c r="H77" t="s">
         <v>97</v>
       </c>
-      <c r="I48" s="4" t="s">
+      <c r="I77" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="J48" s="4" t="s">
+      <c r="J77" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="K48" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B50" s="4"/>
-    </row>
-    <row r="51" spans="2:9" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="B51" s="4" t="s">
+      <c r="K77" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B79" s="4"/>
+    </row>
+    <row r="80" spans="1:11" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="B80" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="I51" t="s">
+      <c r="I80" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="I52" t="s">
+    <row r="81" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I81" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="I53" t="s">
+    <row r="82" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I82" t="s">
         <v>110</v>
       </c>
     </row>

</xml_diff>